<commit_message>
Update PM-LL & PM_Q&A
</commit_message>
<xml_diff>
--- a/Improgress/PM-Lesson-Learned_Ver1.0.xlsx
+++ b/Improgress/PM-Lesson-Learned_Ver1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Capstone-Project\Improgress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/Capstone-Project/Improgress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F67098-620B-487B-A95D-E5E03A66E572}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9A3F8C-CB9A-924C-8624-C8FBA07A3B6D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5F73FFBD-5C3A-4814-BCBC-28C9706C53DD}"/>
+    <workbookView xWindow="-120" yWindow="460" windowWidth="20740" windowHeight="11320" activeTab="5" xr2:uid="{5F73FFBD-5C3A-4814-BCBC-28C9706C53DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision History" sheetId="10" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Trương Quang Vương" sheetId="8" r:id="rId7"/>
     <sheet name="Phạm Quốc Nhân" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="68">
   <si>
     <r>
       <t xml:space="preserve">
@@ -246,12 +246,36 @@
   <si>
     <t>Create lesson learned</t>
   </si>
+  <si>
+    <t xml:space="preserve">Vai trò của tôi trong dự án là Coder. Tôi đảm nhiệm về code website và một số tài liệu liên quan.			</t>
+  </si>
+  <si>
+    <t>Sử dụng framework tốt, ý thức và có tránh nhiệm với nhóm</t>
+  </si>
+  <si>
+    <t>Khả năng xử lý công việc chưa tốt</t>
+  </si>
+  <si>
+    <t>Học hỏi thêm nhiều kiến thức về lập trình</t>
+  </si>
+  <si>
+    <t>Hiểu rõ chuyên sâu về lập trình website</t>
+  </si>
+  <si>
+    <t>Kỹ năng làm việc nhóm rất quan trọng</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>Có ý thức làm việc của từng thành viên, không đun đẩy trách nhiệm.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,7 +872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -904,6 +928,111 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -922,24 +1051,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -952,6 +1063,48 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -977,48 +1130,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1072,93 +1183,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1245,7 +1272,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1543,397 +1570,397 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC71E0BD-B254-4FEA-82DF-AA86120254C9}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="12" max="12" width="13.85546875" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:15" ht="16" thickBot="1">
+      <c r="A1" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="78"/>
-    </row>
-    <row r="3" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="79"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="84" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+    </row>
+    <row r="2" spans="1:15" ht="16" thickBot="1">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="20"/>
+    </row>
+    <row r="3" spans="1:15" ht="35" thickBot="1">
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="M3" s="85" t="s">
+      <c r="M3" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="86"/>
-      <c r="O3" s="87"/>
-    </row>
-    <row r="4" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="79"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="88" t="s">
+      <c r="N3" s="42"/>
+      <c r="O3" s="24"/>
+    </row>
+    <row r="4" spans="1:15" ht="18" thickBot="1">
+      <c r="A4" s="38"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="85" t="s">
+      <c r="M4" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-    </row>
-    <row r="5" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="79"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="84" t="s">
+      <c r="N4" s="42"/>
+      <c r="O4" s="24"/>
+    </row>
+    <row r="5" spans="1:15" ht="18" thickBot="1">
+      <c r="A5" s="38"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="85" t="s">
+      <c r="M5" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="N5" s="86"/>
-      <c r="O5" s="87"/>
-    </row>
-    <row r="6" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="79"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="88" t="s">
+      <c r="N5" s="42"/>
+      <c r="O5" s="24"/>
+    </row>
+    <row r="6" spans="1:15" ht="18" thickBot="1">
+      <c r="A6" s="38"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="85" t="s">
+      <c r="M6" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="86"/>
-      <c r="O6" s="87"/>
-    </row>
-    <row r="7" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="79"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="84" t="s">
+      <c r="N6" s="42"/>
+      <c r="O6" s="24"/>
+    </row>
+    <row r="7" spans="1:15" ht="35" thickBot="1">
+      <c r="A7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="89">
+      <c r="M7" s="43">
         <v>43994</v>
       </c>
-      <c r="N7" s="90"/>
-      <c r="O7" s="87"/>
-    </row>
-    <row r="8" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="79"/>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="87"/>
-      <c r="N8" s="87"/>
-      <c r="O8" s="87"/>
-    </row>
-    <row r="9" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="79"/>
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="87"/>
-      <c r="N9" s="87"/>
-      <c r="O9" s="87"/>
-    </row>
-    <row r="10" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="91"/>
-      <c r="M10" s="91"/>
-      <c r="N10" s="91"/>
-      <c r="O10" s="91"/>
-    </row>
-    <row r="11" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="79"/>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="83"/>
-      <c r="L11" s="92" t="s">
+      <c r="N7" s="44"/>
+      <c r="O7" s="24"/>
+    </row>
+    <row r="8" spans="1:15" ht="17" thickBot="1">
+      <c r="A8" s="38"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+    </row>
+    <row r="9" spans="1:15" ht="17" thickBot="1">
+      <c r="A9" s="38"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+    </row>
+    <row r="10" spans="1:15" ht="17" thickBot="1">
+      <c r="A10" s="38"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+    </row>
+    <row r="11" spans="1:15" ht="17" thickBot="1">
+      <c r="A11" s="38"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="M11" s="93"/>
-      <c r="N11" s="93"/>
-      <c r="O11" s="94"/>
-    </row>
-    <row r="12" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="79"/>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="95" t="s">
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="47"/>
+    </row>
+    <row r="12" spans="1:15" ht="18" thickBot="1">
+      <c r="A12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="M12" s="95" t="s">
+      <c r="M12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N12" s="95" t="s">
+      <c r="N12" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="O12" s="95" t="s">
+      <c r="O12" s="27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="79"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="83"/>
-      <c r="L13" s="96" t="s">
+    <row r="13" spans="1:15" ht="35" thickBot="1">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="M13" s="97">
+      <c r="M13" s="29">
         <v>43994</v>
       </c>
-      <c r="N13" s="98" t="s">
+      <c r="N13" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="O13" s="96" t="s">
+      <c r="O13" s="28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="79"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="83"/>
-      <c r="L14" s="99"/>
-      <c r="M14" s="100"/>
-      <c r="N14" s="100"/>
-      <c r="O14" s="100"/>
-    </row>
-    <row r="15" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="79"/>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="99"/>
-      <c r="M15" s="100"/>
-      <c r="N15" s="100"/>
-      <c r="O15" s="100"/>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="79"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="83"/>
-      <c r="L16" s="101"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="102"/>
-      <c r="O16" s="102"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="79"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="83"/>
-      <c r="L17" s="101"/>
-      <c r="M17" s="102"/>
-      <c r="N17" s="102"/>
-      <c r="O17" s="102"/>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="79"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="101"/>
-      <c r="M18" s="102"/>
-      <c r="N18" s="102"/>
-      <c r="O18" s="102"/>
-    </row>
-    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="79"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="80"/>
-      <c r="I19" s="80"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="83"/>
-      <c r="L19" s="101"/>
-      <c r="M19" s="102"/>
-      <c r="N19" s="102"/>
-      <c r="O19" s="102"/>
-    </row>
-    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="83"/>
-      <c r="L20" s="101"/>
-      <c r="M20" s="102"/>
-      <c r="N20" s="102"/>
-      <c r="O20" s="102"/>
+    <row r="14" spans="1:15" ht="17" thickBot="1">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+    </row>
+    <row r="15" spans="1:15" ht="17" thickBot="1">
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+    </row>
+    <row r="16" spans="1:15" ht="16" thickBot="1">
+      <c r="A16" s="38"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+    </row>
+    <row r="17" spans="1:15" ht="16" thickBot="1">
+      <c r="A17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+    </row>
+    <row r="18" spans="1:15" ht="16" thickBot="1">
+      <c r="A18" s="38"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+    </row>
+    <row r="19" spans="1:15" ht="16" thickBot="1">
+      <c r="A19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+    </row>
+    <row r="20" spans="1:15" ht="16" thickBot="1">
+      <c r="A20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1957,42 +1984,42 @@
       <selection activeCell="C9" sqref="C9:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:6" ht="91.5" customHeight="1" thickBot="1">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:6" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
+      <c r="A2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+    </row>
+    <row r="3" spans="1:6" ht="18" customHeight="1" thickBot="1"/>
+    <row r="4" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A4" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="57"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="59"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -2006,76 +2033,76 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+    <row r="6" spans="1:6" ht="18" customHeight="1" thickBot="1"/>
+    <row r="7" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A7" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="B7" s="57"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="59"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A8" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="25" t="str">
+      <c r="B8" s="51"/>
+      <c r="C8" s="48" t="str">
         <f>'Huỳnh Tuấn Đạt'!C1:E1</f>
         <v>Huỳnh Tuấn Đạt</v>
       </c>
-      <c r="D8" s="26"/>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="25" t="str">
+      <c r="D8" s="49"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A9" s="52"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="48" t="str">
         <f>'Trịnh Thị Như Phương'!C1:E1</f>
         <v>Trịnh Thị Như Phương</v>
       </c>
-      <c r="D9" s="26"/>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="25" t="str">
+      <c r="D9" s="49"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A10" s="52"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="48" t="str">
         <f>'Nguyễn Anh Minh'!C1:E1</f>
         <v>Nguyễn Anh Minh</v>
       </c>
-      <c r="D10" s="26"/>
-    </row>
-    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="25" t="str">
+      <c r="D10" s="49"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A11" s="52"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="48" t="str">
         <f>'Trương Quang Vương'!C1:E1</f>
         <v>Trương Quang Vương</v>
       </c>
-      <c r="D11" s="26"/>
-    </row>
-    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="25" t="str">
+      <c r="D11" s="49"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A12" s="52"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="48" t="str">
         <f>'Phạm Quốc Nhân'!C1:E1</f>
         <v>Phạm Quốc Nhân</v>
       </c>
-      <c r="D12" s="26"/>
+      <c r="D12" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="A8:B12"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2090,21 +2117,21 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="146.28515625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="146.33203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:2" ht="29.25" customHeight="1">
+      <c r="A1" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="31"/>
-    </row>
-    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="60"/>
+    </row>
+    <row r="2" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="3" spans="1:2" ht="18.75" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -2112,97 +2139,97 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="32"/>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="61"/>
+    </row>
+    <row r="5" spans="1:2" ht="18.75" customHeight="1">
       <c r="A5" s="7">
         <v>1</v>
       </c>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1">
       <c r="A6" s="7">
         <v>2</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1">
       <c r="A7" s="7">
         <v>3</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A8" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="32"/>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="61"/>
+    </row>
+    <row r="9" spans="1:2" ht="18.75" customHeight="1">
       <c r="A9" s="7"/>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1">
       <c r="A10" s="7"/>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1">
       <c r="A11" s="7"/>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A12" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="34"/>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="63"/>
+    </row>
+    <row r="13" spans="1:2" ht="18.75" customHeight="1">
       <c r="A13" s="7"/>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1">
       <c r="A14" s="7"/>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1">
       <c r="A15" s="7"/>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1">
       <c r="A16" s="7"/>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A17" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="34"/>
-    </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="63"/>
+    </row>
+    <row r="18" spans="1:2" ht="18.75" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="18.75" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="18.75" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="18.75" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="18.75" customHeight="1">
       <c r="A22" s="7"/>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="18.75" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="6"/>
     </row>
@@ -2227,93 +2254,93 @@
       <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="9" customWidth="1"/>
-    <col min="2" max="5" width="39.7109375" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.83203125" style="9" customWidth="1"/>
+    <col min="2" max="5" width="39.6640625" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A1" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-    </row>
-    <row r="2" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+    </row>
+    <row r="2" spans="1:5" ht="9" customHeight="1">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A3" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A4" s="70"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A5" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A6" s="69"/>
       <c r="B6" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="48"/>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="E6" s="67"/>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A7" s="70"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="D7" s="74"/>
+      <c r="E7" s="75"/>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A8" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A9" s="76"/>
       <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
@@ -2327,8 +2354,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+    <row r="10" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A10" s="77"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -2336,17 +2363,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:A4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2361,93 +2388,93 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="9" customWidth="1"/>
-    <col min="2" max="5" width="39.7109375" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.83203125" style="9" customWidth="1"/>
+    <col min="2" max="5" width="39.6640625" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A1" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-    </row>
-    <row r="2" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+    </row>
+    <row r="2" spans="1:5" ht="9" customHeight="1">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A3" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A4" s="70"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A5" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A6" s="69"/>
       <c r="B6" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="48"/>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="E6" s="67"/>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A7" s="70"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="D7" s="74"/>
+      <c r="E7" s="75"/>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A8" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A9" s="76"/>
       <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
@@ -2461,8 +2488,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+    <row r="10" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A10" s="77"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -2491,116 +2518,132 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C46D46-684F-4EBD-9267-7EACD9942B13}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="9" customWidth="1"/>
-    <col min="2" max="5" width="39.7109375" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.83203125" style="9" customWidth="1"/>
+    <col min="2" max="5" width="39.6640625" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A1" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-    </row>
-    <row r="2" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+    </row>
+    <row r="2" spans="1:5" ht="9" customHeight="1">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A3" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+    </row>
+    <row r="4" spans="1:5" ht="14">
+      <c r="A4" s="70"/>
+      <c r="B4" s="78" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A5" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A6" s="69"/>
       <c r="B6" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="48"/>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="E6" s="67"/>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" s="70"/>
+      <c r="B7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="102" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="103"/>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A8" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="14"/>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
-      <c r="B9" s="15" t="s">
+      <c r="C8" s="90"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A9" s="76"/>
+      <c r="B9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10" s="77"/>
+      <c r="B10" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2629,93 +2672,93 @@
       <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="9" customWidth="1"/>
-    <col min="2" max="5" width="39.7109375" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.83203125" style="9" customWidth="1"/>
+    <col min="2" max="5" width="39.6640625" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A1" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-    </row>
-    <row r="2" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+    </row>
+    <row r="2" spans="1:5" ht="9" customHeight="1">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A3" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A4" s="70"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A5" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A6" s="69"/>
       <c r="B6" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="48"/>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="E6" s="67"/>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A7" s="70"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="D7" s="74"/>
+      <c r="E7" s="75"/>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A8" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A9" s="76"/>
       <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
@@ -2729,8 +2772,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+    <row r="10" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A10" s="77"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -2763,101 +2806,101 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="9" customWidth="1"/>
-    <col min="2" max="5" width="39.7109375" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.83203125" style="9" customWidth="1"/>
+    <col min="2" max="5" width="39.6640625" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A1" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-    </row>
-    <row r="2" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+    </row>
+    <row r="2" spans="1:5" ht="9" customHeight="1">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A3" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63"/>
-      <c r="B4" s="66" t="s">
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A4" s="92"/>
+      <c r="B4" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A5" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="68"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A6" s="97"/>
       <c r="B6" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="72"/>
-    </row>
-    <row r="7" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
+      <c r="E6" s="101"/>
+    </row>
+    <row r="7" spans="1:5" ht="76.5" customHeight="1">
+      <c r="A7" s="92"/>
       <c r="B7" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="73" t="s">
+      <c r="D7" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="74"/>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+      <c r="E7" s="103"/>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A8" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="62"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="91"/>
       <c r="E8" s="18"/>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A9" s="87"/>
       <c r="B9" s="16" t="s">
         <v>7</v>
       </c>
@@ -2871,8 +2914,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="57" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
+    <row r="10" spans="1:5" ht="45">
+      <c r="A10" s="88"/>
       <c r="B10" s="17" t="s">
         <v>37</v>
       </c>

</xml_diff>